<commit_message>
ComputerPage.java is almost complete.
</commit_message>
<xml_diff>
--- a/src/main/java/SIT_Automation_TestData_v1.xlsx
+++ b/src/main/java/SIT_Automation_TestData_v1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -103,10 +103,7 @@
     <t>GCL_AUT02</t>
   </si>
   <si>
-    <t>pressComputerTab</t>
-  </si>
-  <si>
-    <t>GCL_AUT03</t>
+    <t>purchaseCheapComputer</t>
   </si>
   <si>
     <t>SheetName</t>
@@ -2083,7 +2080,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -2175,15 +2172,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="16">
         <f>COUNTA(TestData!$A:$A)-1</f>
@@ -2192,7 +2189,7 @@
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="16">
         <f>COUNTA(#REF!)-1</f>
@@ -2201,7 +2198,7 @@
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="16">
         <f>COUNTA(#REF!)-1</f>
@@ -2210,7 +2207,7 @@
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="16">
         <f>COUNTA(LoginTests!$A:$A)-1</f>
@@ -2219,7 +2216,7 @@
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="16">
         <f>COUNTA(HomePageTests!$A:$A)-1</f>
@@ -2228,7 +2225,7 @@
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="16">
         <f>COUNTA(#REF!)-1</f>
@@ -2237,7 +2234,7 @@
     </row>
     <row r="8">
       <c r="A8" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="16">
         <f>COUNTA(#REF!)-1</f>
@@ -2246,7 +2243,7 @@
     </row>
     <row r="9">
       <c r="A9" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="16">
         <f>COUNTA(#REF!)-1</f>
@@ -2255,7 +2252,7 @@
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="16">
         <f>COUNTA(#REF!)-1</f>
@@ -2264,7 +2261,7 @@
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="16">
         <f>COUNTA(#REF!) -1</f>
@@ -2273,7 +2270,7 @@
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="16">
         <f>COUNTA(#REF!)-1</f>
@@ -2282,7 +2279,7 @@
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="16">
         <f>COUNTA(#REF!)-1</f>
@@ -2291,7 +2288,7 @@
     </row>
     <row r="14">
       <c r="A14" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="16">
         <f>COUNTA(#REF!)-1</f>
@@ -2300,7 +2297,7 @@
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="16">
         <v>4</v>
@@ -2308,7 +2305,7 @@
     </row>
     <row r="16">
       <c r="A16" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="16">
         <v>5</v>
@@ -2316,7 +2313,7 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="17">
         <f>SUM(B2:B16)</f>

</xml_diff>

<commit_message>
Added digital download page module
Added digital download implementation
added digital download test
modified .properties files
</commit_message>
<xml_diff>
--- a/src/main/java/SIT_Automation_TestData_v1.xlsx
+++ b/src/main/java/SIT_Automation_TestData_v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrbee\eclipse-workspace\demo-web-shop\src\main\java\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mrbee\eclipse-workspace\Main\src\main\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6D29F3-0745-4A3B-9CE4-BC6FF3AA83FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F1B681-B168-47E9-AB4D-353441A32E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="928" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="928" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>DWS_AUTO2</t>
+  </si>
+  <si>
+    <t>selectItem</t>
   </si>
 </sst>
 </file>
@@ -1880,8 +1883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1980,6 +1983,9 @@
       <c r="M3" s="19"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="G4" s="20"/>
@@ -2007,7 +2013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -2076,7 +2082,7 @@
       </c>
       <c r="B7" s="14">
         <f>COUNTA(DigitalPageTest!$A:$A)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2164,7 +2170,7 @@
       </c>
       <c r="B17" s="15">
         <f>SUM(B2:B16)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>